<commit_message>
fonts and fills, moved credentials file
# Conflicts:
#	spreadsheets/google_sheets/create_gsheet.py
</commit_message>
<xml_diff>
--- a/spreadsheets/excel/Employee Ratings.xlsx
+++ b/spreadsheets/excel/Employee Ratings.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -463,6 +463,11 @@
           <t>Q4 Rating</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Average Rating</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,6 +486,10 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(B2:E2)</f>
+        <v/>
       </c>
     </row>
     <row r="3">

</xml_diff>